<commit_message>
create pph 21 manfaat
</commit_message>
<xml_diff>
--- a/public/files/contoh rapel manfaat.xlsx
+++ b/public/files/contoh rapel manfaat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\rohman\1 EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6068B84-D731-45F7-9787-E12C8D504CEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B2E1C4-A131-4E3D-BCBF-CCFA27995622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0E19FFF5-2BAF-4F21-812C-E6CCD4CE39B2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Jenis Transaksi</t>
   </si>
@@ -78,15 +78,9 @@
     <t>AIB</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>AIH</t>
   </si>
   <si>
-    <t>DENI</t>
-  </si>
-  <si>
     <t>tes ubah lagi</t>
   </si>
   <si>
@@ -105,16 +99,22 @@
     <t>Extra Manfaat 4</t>
   </si>
   <si>
-    <t>AIJ</t>
-  </si>
-  <si>
-    <t>ADIT</t>
-  </si>
-  <si>
-    <t>ASEP</t>
-  </si>
-  <si>
-    <t>ILHAM</t>
+    <t>ARDI</t>
+  </si>
+  <si>
+    <t>DANI</t>
+  </si>
+  <si>
+    <t>ALIM</t>
+  </si>
+  <si>
+    <t>Extra Manfaat 5</t>
+  </si>
+  <si>
+    <t>AIG</t>
+  </si>
+  <si>
+    <t>AIK</t>
   </si>
 </sst>
 </file>
@@ -575,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB0650C-83BC-43B8-BFD5-EA223C6539B0}">
-  <dimension ref="B4:N13"/>
+  <dimension ref="B4:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +681,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="2">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F10" s="3">
         <v>44080</v>
@@ -690,10 +690,10 @@
         <v>212</v>
       </c>
       <c r="H10" s="2">
-        <v>292900</v>
+        <v>1000001</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J10" s="3">
         <v>43957</v>
@@ -708,7 +708,7 @@
         <v>2000000</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -716,13 +716,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F11" s="3">
         <v>40948</v>
@@ -731,10 +731,10 @@
         <v>211</v>
       </c>
       <c r="H11" s="2">
-        <v>435643</v>
+        <v>1000002</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J11" s="3">
         <v>43957</v>
@@ -749,7 +749,7 @@
         <v>444444</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -757,13 +757,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F12" s="3">
         <v>40948</v>
@@ -772,10 +772,10 @@
         <v>222</v>
       </c>
       <c r="H12" s="2">
-        <v>2</v>
+        <v>1000003</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J12" s="3">
         <v>43957</v>
@@ -790,7 +790,7 @@
         <v>444444</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F13" s="3">
         <v>40948</v>
@@ -813,10 +813,10 @@
         <v>222</v>
       </c>
       <c r="H13" s="2">
-        <v>4341</v>
+        <v>1000004</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J13" s="3">
         <v>43957</v>
@@ -831,7 +831,48 @@
         <v>444444</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2">
+        <v>42</v>
+      </c>
+      <c r="F14" s="3">
+        <v>40948</v>
+      </c>
+      <c r="G14" s="2">
+        <v>222</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1000005</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="3">
+        <v>43957</v>
+      </c>
+      <c r="K14" s="3">
+        <v>43977</v>
+      </c>
+      <c r="L14" s="2">
+        <v>222222</v>
+      </c>
+      <c r="M14" s="2">
+        <v>444444</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>